<commit_message>
dunno, touched a file
</commit_message>
<xml_diff>
--- a/docs/trainers.xlsx
+++ b/docs/trainers.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhanney\dev\zwiftalizer\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mike.hanney\dev\zwiftalizer\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -258,7 +258,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -274,7 +274,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,6 +284,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -300,11 +306,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,7 +673,7 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>22</v>
       </c>
       <c r="D2" t="s">
@@ -686,7 +693,7 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>0</v>
       </c>
       <c r="D3" t="s">
@@ -709,7 +716,7 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>0</v>
       </c>
       <c r="D4" t="s">
@@ -732,7 +739,7 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>18</v>
       </c>
       <c r="D5" t="s">
@@ -751,7 +758,7 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <v>21</v>
       </c>
       <c r="D6" t="s">
@@ -881,7 +888,7 @@
       <c r="B14" t="s">
         <v>20</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="4">
         <v>320</v>
       </c>
       <c r="D14" t="s">
@@ -952,7 +959,7 @@
       <c r="B18" t="s">
         <v>32</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <v>2010</v>
       </c>
       <c r="D18" t="s">
@@ -975,7 +982,7 @@
       <c r="B19" t="s">
         <v>32</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="4">
         <v>2400</v>
       </c>
       <c r="D19" t="s">
@@ -995,7 +1002,7 @@
       <c r="B20" t="s">
         <v>32</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="4">
         <v>2240</v>
       </c>
       <c r="D20" t="s">
@@ -1012,7 +1019,7 @@
       <c r="B21" t="s">
         <v>32</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="4">
         <v>2060</v>
       </c>
       <c r="D21" t="s">
@@ -1029,7 +1036,7 @@
       <c r="B22" t="s">
         <v>32</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="4">
         <v>2080</v>
       </c>
       <c r="D22" t="s">
@@ -1046,7 +1053,7 @@
       <c r="B23" t="s">
         <v>32</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="4">
         <v>2180</v>
       </c>
       <c r="D23" t="s">
@@ -1063,7 +1070,7 @@
       <c r="B24" t="s">
         <v>32</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="4">
         <v>2780</v>
       </c>
       <c r="D24" t="s">
@@ -1080,7 +1087,7 @@
       <c r="B25" t="s">
         <v>32</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="4">
         <v>2800</v>
       </c>
       <c r="D25" t="s">
@@ -1103,7 +1110,7 @@
       <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="4">
         <v>2900</v>
       </c>
       <c r="D26" t="s">
@@ -1123,7 +1130,7 @@
       <c r="B27" t="s">
         <v>32</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="4">
         <v>1</v>
       </c>
       <c r="D27" t="s">
@@ -1146,7 +1153,7 @@
       <c r="B28" t="s">
         <v>40</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="4">
         <v>1</v>
       </c>
       <c r="D28" t="s">
@@ -1169,7 +1176,7 @@
       <c r="B29" t="s">
         <v>40</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="4">
         <v>16</v>
       </c>
       <c r="D29" t="s">
@@ -1216,8 +1223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,7 +1264,7 @@
       <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>1380</v>
       </c>
       <c r="D2" t="s">
@@ -1271,7 +1278,7 @@
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>1381</v>
       </c>
       <c r="D3" t="s">
@@ -1288,7 +1295,7 @@
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>2079</v>
       </c>
       <c r="D4" t="s">
@@ -1305,7 +1312,7 @@
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>2161</v>
       </c>
       <c r="D5" t="s">
@@ -1322,7 +1329,7 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <v>2162</v>
       </c>
       <c r="D6" t="s">
@@ -1339,7 +1346,7 @@
       <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <v>7</v>
       </c>
       <c r="D7" t="s">
@@ -1353,7 +1360,7 @@
       <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <v>272</v>
       </c>
       <c r="D8" t="s">
@@ -1373,7 +1380,7 @@
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <v>4096</v>
       </c>
       <c r="D9" t="s">
@@ -1393,7 +1400,7 @@
       <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
         <v>288</v>
       </c>
       <c r="D10" t="s">
@@ -1413,7 +1420,7 @@
       <c r="B11" t="s">
         <v>27</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="4">
         <v>1031</v>
       </c>
       <c r="D11" t="s">
@@ -1433,7 +1440,7 @@
       <c r="B12" t="s">
         <v>30</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <v>1</v>
       </c>
       <c r="D12" t="s">
@@ -1505,6 +1512,9 @@
       </c>
       <c r="D17" t="s">
         <v>69</v>
+      </c>
+      <c r="E17">
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added more power sources specs
</commit_message>
<xml_diff>
--- a/docs/trainers.xlsx
+++ b/docs/trainers.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mike.hanney\dev\zwiftalizer\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhanney\dev\zwiftalizer\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="Trainers" sheetId="1" r:id="rId1"/>
     <sheet name="Powermeters" sheetId="2" r:id="rId2"/>
+    <sheet name="CLUT" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="106">
   <si>
     <t>ManufacturerId</t>
   </si>
@@ -210,18 +211,6 @@
     <t>Indoor Cycle</t>
   </si>
   <si>
-    <t>Real Turbo Muin (ANT+)</t>
-  </si>
-  <si>
-    <t>Real Axiom (ANT+)</t>
-  </si>
-  <si>
-    <t>Real Tour (ANT+)</t>
-  </si>
-  <si>
-    <t>Real Power (ANT+)</t>
-  </si>
-  <si>
     <t>Left Only</t>
   </si>
   <si>
@@ -253,13 +242,115 @@
   </si>
   <si>
     <t>Phantom 5</t>
+  </si>
+  <si>
+    <t>Max Power</t>
+  </si>
+  <si>
+    <t>9913 is BTLE</t>
+  </si>
+  <si>
+    <t>9481 is BTLE</t>
+  </si>
+  <si>
+    <t>Real Axiom</t>
+  </si>
+  <si>
+    <t>Real Axiom B+</t>
+  </si>
+  <si>
+    <t>Real Tour</t>
+  </si>
+  <si>
+    <t>Real Tour B+</t>
+  </si>
+  <si>
+    <t>Real Turbo Muin</t>
+  </si>
+  <si>
+    <t>Real Turbo Muin B+</t>
+  </si>
+  <si>
+    <t>Turbo Roteo Smart B+</t>
+  </si>
+  <si>
+    <t>Kinetic</t>
+  </si>
+  <si>
+    <t>Smart Control Power Unit</t>
+  </si>
+  <si>
+    <t>Real E-motion rollers</t>
+  </si>
+  <si>
+    <t>Real E-motion B+  rollers</t>
+  </si>
+  <si>
+    <t>SKU</t>
+  </si>
+  <si>
+    <t>Rock and Roll Smart Control</t>
+  </si>
+  <si>
+    <t>Road Machine Smart Control</t>
+  </si>
+  <si>
+    <t>#62b5e5</t>
+  </si>
+  <si>
+    <t>#003479</t>
+  </si>
+  <si>
+    <t>#ffd403</t>
+  </si>
+  <si>
+    <t>#62b800</t>
+  </si>
+  <si>
+    <t>#dc1f1f</t>
+  </si>
+  <si>
+    <t>#1d1d1d</t>
+  </si>
+  <si>
+    <t>#1285c7</t>
+  </si>
+  <si>
+    <t>#e32525</t>
+  </si>
+  <si>
+    <t>#b1343a</t>
+  </si>
+  <si>
+    <t>#0079c1</t>
+  </si>
+  <si>
+    <t>#b4cc64</t>
+  </si>
+  <si>
+    <t>#d0112b</t>
+  </si>
+  <si>
+    <t>#000000</t>
+  </si>
+  <si>
+    <t>#383838</t>
+  </si>
+  <si>
+    <t>Precision Pro</t>
+  </si>
+  <si>
+    <t>Infocrank </t>
+  </si>
+  <si>
+    <t>Verve</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,8 +364,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,6 +395,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -306,12 +414,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,9 +752,11 @@
     <col min="5" max="5" width="16.140625" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -665,8 +778,11 @@
       <c r="G1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>67</v>
       </c>
@@ -686,7 +802,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>86</v>
       </c>
@@ -709,7 +825,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>86</v>
       </c>
@@ -732,7 +848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>86</v>
       </c>
@@ -751,7 +867,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>86</v>
       </c>
@@ -774,7 +890,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>86</v>
       </c>
@@ -791,7 +907,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>86</v>
       </c>
@@ -808,7 +924,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>86</v>
       </c>
@@ -825,7 +941,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>86</v>
       </c>
@@ -834,26 +950,29 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>79</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>86</v>
-      </c>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>80</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>86</v>
       </c>
@@ -862,354 +981,627 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>86</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="4">
-        <v>320</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C14" s="1"/>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="F14">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>9</v>
-      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="F15">
-        <v>0.03</v>
-      </c>
-      <c r="G15">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>9</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C18" s="1"/>
+      <c r="D18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
+      <c r="D19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="1"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="1"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="1">
+        <v>6200</v>
+      </c>
+      <c r="D22" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="1">
+        <v>6100</v>
+      </c>
+      <c r="D23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="1">
+        <v>6000</v>
+      </c>
+      <c r="D24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C25" s="1"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="4">
+        <v>320</v>
+      </c>
+      <c r="D26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>0.03</v>
+      </c>
+      <c r="G26">
+        <v>0.2</v>
+      </c>
+      <c r="H26">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>0.03</v>
+      </c>
+      <c r="G27">
+        <v>0.15</v>
+      </c>
+      <c r="H27" s="3">
+        <v>1500</v>
+      </c>
+      <c r="J27" s="6">
+        <v>9920</v>
+      </c>
+      <c r="K27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>9</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="2">
+        <v>1000</v>
+      </c>
+      <c r="I28" t="s">
+        <v>74</v>
+      </c>
+      <c r="J28" s="5">
+        <v>9480</v>
+      </c>
+      <c r="K28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>9</v>
+      </c>
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="2">
+        <v>1000</v>
+      </c>
+      <c r="I29" t="s">
+        <v>73</v>
+      </c>
+      <c r="J29" s="3">
+        <v>9912</v>
+      </c>
+      <c r="K29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C30" s="3"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>89</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B31" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C31" s="4">
         <v>2010</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D31" t="s">
         <v>33</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
         <v>0.05</v>
       </c>
-      <c r="G18">
+      <c r="G31">
+        <v>0.2</v>
+      </c>
+      <c r="H31">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>89</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="4">
+        <v>2400</v>
+      </c>
+      <c r="D32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0.1</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>89</v>
+      </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="4">
+        <v>2240</v>
+      </c>
+      <c r="D33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>0.1</v>
+      </c>
+      <c r="G33">
+        <v>0.06</v>
+      </c>
+      <c r="H33">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>89</v>
+      </c>
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="4">
+        <v>2060</v>
+      </c>
+      <c r="D34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>0.05</v>
+      </c>
+      <c r="G34">
+        <v>0.2</v>
+      </c>
+      <c r="H34">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>89</v>
+      </c>
+      <c r="B35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="4">
+        <v>2080</v>
+      </c>
+      <c r="D35" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>0.05</v>
+      </c>
+      <c r="G35">
+        <v>0.2</v>
+      </c>
+      <c r="H35">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>89</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="4">
+        <v>2180</v>
+      </c>
+      <c r="D36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>0.1</v>
+      </c>
+      <c r="G36">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="H36">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>89</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B37" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="4">
-        <v>2400</v>
-      </c>
-      <c r="D19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="C37" s="4">
+        <v>2780</v>
+      </c>
+      <c r="D37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>0.1</v>
+      </c>
+      <c r="G37">
+        <v>0.15</v>
+      </c>
+      <c r="H37">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>89</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B38" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="4">
-        <v>2240</v>
-      </c>
-      <c r="D20" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="C38" s="4">
+        <v>2800</v>
+      </c>
+      <c r="D38" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>0.02</v>
+      </c>
+      <c r="G38">
+        <v>0.25</v>
+      </c>
+      <c r="H38">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>89</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B39" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="4">
-        <v>2060</v>
-      </c>
-      <c r="D21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="C39" s="4">
+        <v>2900</v>
+      </c>
+      <c r="D39" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>0.05</v>
+      </c>
+      <c r="G39">
+        <v>0.1</v>
+      </c>
+      <c r="H39">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>89</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B40" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="4">
-        <v>2080</v>
-      </c>
-      <c r="D22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>89</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C40" s="4">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>38</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>0.02</v>
+      </c>
+      <c r="G40">
+        <v>0.25</v>
+      </c>
+      <c r="H40">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>32</v>
       </c>
-      <c r="C23" s="4">
-        <v>2180</v>
-      </c>
-      <c r="D23" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>89</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="B42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" s="4">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>41</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>0.03</v>
+      </c>
+      <c r="G42">
+        <v>0.2</v>
+      </c>
+      <c r="H42">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>32</v>
       </c>
-      <c r="C24" s="4">
-        <v>2780</v>
-      </c>
-      <c r="D24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>89</v>
-      </c>
-      <c r="B25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="4">
-        <v>2800</v>
-      </c>
-      <c r="D25" t="s">
-        <v>38</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>0.01</v>
-      </c>
-      <c r="G25">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>89</v>
-      </c>
-      <c r="B26" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="4">
-        <v>2900</v>
-      </c>
-      <c r="D26" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
+      <c r="B43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="4">
+        <v>16</v>
+      </c>
+      <c r="D43" t="s">
+        <v>42</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>89</v>
-      </c>
-      <c r="B27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="4">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>0.01</v>
-      </c>
-      <c r="G27">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>32</v>
-      </c>
-      <c r="B28" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="4">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
-        <v>41</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="F28">
-        <v>0.03</v>
-      </c>
-      <c r="G28">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>32</v>
-      </c>
-      <c r="B29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="4">
-        <v>16</v>
-      </c>
-      <c r="D29" t="s">
-        <v>42</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="F29">
+      <c r="G43">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>30</v>
+      </c>
+      <c r="B44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" s="1"/>
+      <c r="D44" t="s">
+        <v>47</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
         <v>0.05</v>
       </c>
-      <c r="G29">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>30</v>
-      </c>
-      <c r="B30" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" t="s">
-        <v>47</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0.05</v>
-      </c>
-      <c r="G30">
+      <c r="G44">
         <v>0</v>
       </c>
     </row>
@@ -1221,10 +1613,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,7 +1646,7 @@
         <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1264,7 +1656,7 @@
       <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="2">
         <v>1380</v>
       </c>
       <c r="D2" t="s">
@@ -1278,7 +1670,7 @@
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="2">
         <v>1381</v>
       </c>
       <c r="D3" t="s">
@@ -1295,7 +1687,7 @@
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="2">
         <v>2079</v>
       </c>
       <c r="D4" t="s">
@@ -1312,7 +1704,7 @@
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>2161</v>
       </c>
       <c r="D5" t="s">
@@ -1329,7 +1721,7 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="2">
         <v>2162</v>
       </c>
       <c r="D6" t="s">
@@ -1346,28 +1738,26 @@
       <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="2">
         <v>7</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
       </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="4">
-        <v>272</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C8" s="2"/>
       <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8">
-        <v>0.02</v>
+        <v>103</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1380,11 +1770,11 @@
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="4">
-        <v>4096</v>
+      <c r="C9" s="2">
+        <v>272</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9">
         <v>0.02</v>
@@ -1400,14 +1790,14 @@
       <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="4">
-        <v>288</v>
+      <c r="C10" s="2">
+        <v>4096</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10">
-        <v>1.4999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1415,19 +1805,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="4">
-        <v>1031</v>
+        <v>20</v>
+      </c>
+      <c r="C11" s="2">
+        <v>288</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E11">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1435,16 +1825,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="4">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1031</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="E12">
+        <v>0.02</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1452,27 +1845,31 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
       </c>
       <c r="D13" t="s">
         <v>29</v>
       </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C14" s="2"/>
       <c r="D14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14">
-        <v>1.4999999999999999E-2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1483,10 +1880,13 @@
         <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E15">
         <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1497,10 +1897,13 @@
         <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E16">
         <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1511,10 +1914,13 @@
         <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E17">
         <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1525,32 +1931,41 @@
         <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E18">
         <v>1.4999999999999999E-2</v>
       </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>263</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E20">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -1561,57 +1976,66 @@
         <v>263</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D21" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="E21">
         <v>0.02</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>60</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>29</v>
+        <v>263</v>
+      </c>
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22">
+        <v>0.02</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>99</v>
-      </c>
-      <c r="B23" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" t="s">
-        <v>74</v>
+        <v>60</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
+        <v>99</v>
+      </c>
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>73</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>56</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1619,19 +2043,216 @@
         <v>57</v>
       </c>
       <c r="D26" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>101</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>59</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>60</v>
       </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>86</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>89</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>69</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>263</v>
+      </c>
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
begin wiring up & rendering powerSources data
</commit_message>
<xml_diff>
--- a/docs/trainers.xlsx
+++ b/docs/trainers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21645" windowHeight="9630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21645" windowHeight="9630" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Trainers" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="108">
   <si>
     <t>ManufacturerId</t>
   </si>
@@ -344,13 +344,19 @@
   </si>
   <si>
     <t>Verve</t>
+  </si>
+  <si>
+    <t>Watteam</t>
+  </si>
+  <si>
+    <t>#0099a8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +378,12 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -414,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -423,6 +435,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,7 +754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
@@ -1615,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2083,7 +2098,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2251,10 +2266,22 @@
         <v>102</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>261</v>
+      </c>
+      <c r="B16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>